<commit_message>
Retrieve HRV Net Turnover from Data File
</commit_message>
<xml_diff>
--- a/src/main/resources/ProviderFiles/HRV/HRV_Data_May.xlsx
+++ b/src/main/resources/ProviderFiles/HRV/HRV_Data_May.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mytabcorp-my.sharepoint.com/personal/jack_gale_tabcorp_com_au/Documents/Desktop/Programs/SiennaSpy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\ReportKisser\src\main\resources\ProviderFiles\HRV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{AA161094-3F0B-4A48-9943-7268C8DF5451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCA6E99E-2507-4874-8B52-1E378CFCCAA8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000BB24F-31CA-4E61-A1CD-25722257BC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1021,7 +1021,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,41 +1188,45 @@
         <v>100</v>
       </c>
       <c r="F6" s="10">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G6" s="7">
         <f>E6-F6</f>
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H6" s="8">
         <f t="shared" ref="H6:H37" si="0">G6/E6</f>
-        <v>0.9</v>
-      </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+        <v>0.88</v>
+      </c>
+      <c r="I6" s="10">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="10">
+        <v>9</v>
+      </c>
       <c r="K6" s="7">
         <f>I6-J6</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="8" t="e">
+        <v>991</v>
+      </c>
+      <c r="L6" s="8">
         <f>K6/I6</f>
-        <v>#DIV/0!</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="M6" s="11">
         <f>E6+I6</f>
-        <v>100</v>
+        <v>1100</v>
       </c>
       <c r="N6" s="11">
         <f>F6+J6</f>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="O6" s="7">
         <f>M6-N6</f>
-        <v>90</v>
+        <v>1079</v>
       </c>
       <c r="P6" s="21">
         <f>O6/M6</f>
-        <v>0.9</v>
+        <v>0.98090909090909095</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -1240,31 +1244,35 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="I7" s="10">
+        <v>999</v>
+      </c>
+      <c r="J7" s="10">
+        <v>76</v>
+      </c>
       <c r="K7" s="7">
         <f t="shared" ref="K7:K251" si="2">I7-J7</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="8" t="e">
+        <v>923</v>
+      </c>
+      <c r="L7" s="8">
         <f t="shared" ref="L7:L251" si="3">K7/I7</f>
-        <v>#DIV/0!</v>
+        <v>0.92392392392392397</v>
       </c>
       <c r="M7" s="11">
         <f t="shared" ref="M7:M70" si="4">E7+I7</f>
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="N7" s="11">
         <f t="shared" ref="N7:N70" si="5">F7+J7</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="O7" s="7">
         <f t="shared" ref="O7:O251" si="6">M7-N7</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="21" t="e">
+        <v>923</v>
+      </c>
+      <c r="P7" s="21">
         <f t="shared" ref="P7:P251" si="7">O7/M7</f>
-        <v>#DIV/0!</v>
+        <v>0.92392392392392397</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -19931,47 +19939,47 @@
       </c>
       <c r="F452" s="23">
         <f>SUM(F6:F451)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G452" s="23">
         <f>SUM(G6:G451)</f>
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H452" s="24">
         <f>G452/E452</f>
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="I452" s="23">
         <f>SUM(I6:I451)</f>
-        <v>0</v>
+        <v>1999</v>
       </c>
       <c r="J452" s="23">
         <f>SUM(J6:J451)</f>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="K452" s="23">
         <f>SUM(K6:K451)</f>
-        <v>0</v>
-      </c>
-      <c r="L452" s="24" t="e">
+        <v>1914</v>
+      </c>
+      <c r="L452" s="24">
         <f t="shared" ref="L452" si="60">K452/I452</f>
-        <v>#DIV/0!</v>
+        <v>0.95747873936968486</v>
       </c>
       <c r="M452" s="23">
         <f>SUM(M6:M451)</f>
-        <v>100</v>
+        <v>2099</v>
       </c>
       <c r="N452" s="23">
         <f>SUM(N6:N451)</f>
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="O452" s="23">
         <f>SUM(O6:O451)</f>
-        <v>90</v>
+        <v>2002</v>
       </c>
       <c r="P452" s="25">
         <f t="shared" ref="P452" si="61">O452/M452</f>
-        <v>0.9</v>
+        <v>0.9537875178656503</v>
       </c>
     </row>
     <row r="453" spans="1:16" x14ac:dyDescent="0.3">
@@ -22463,6 +22471,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003705F7A6F39F6144B366789454E3AC72" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7b3bc03ce25bd98d0408fa6f4c223ae3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="33450450-8063-41a7-930e-2b7960be1731" xmlns:ns4="49ab8040-078f-4f8b-a32d-cb44d602eea9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8904d0a6cdbf637ff5f207e345af05c0" ns3:_="" ns4:_="">
     <xsd:import namespace="33450450-8063-41a7-930e-2b7960be1731"/>
@@ -22679,22 +22702,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC77F13-1EC3-44E7-9088-21F815B56FED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="33450450-8063-41a7-930e-2b7960be1731"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="49ab8040-078f-4f8b-a32d-cb44d602eea9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA0706B-052D-4413-8CC0-96F8BF883E6F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21B982F8-06E0-4935-9AAC-CA7DCF56120B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22711,29 +22744,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FA0706B-052D-4413-8CC0-96F8BF883E6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECC77F13-1EC3-44E7-9088-21F815B56FED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="33450450-8063-41a7-930e-2b7960be1731"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="49ab8040-078f-4f8b-a32d-cb44d602eea9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>